<commit_message>
+ comment on "Aug " in b/n row headers in agenda.xlsx
</commit_message>
<xml_diff>
--- a/data/agenda.xlsx
+++ b/data/agenda.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="0" windowWidth="17440" windowHeight="21040" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="0" windowWidth="28500" windowHeight="21040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Benjamin Best</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin Best:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Agenda looks for Times starting with "Aug " to determine if inserting header.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
   <si>
@@ -250,7 +292,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,6 +332,24 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -718,468 +778,468 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="18" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="3" customFormat="1">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:3" s="3" customFormat="1">
+      <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="2:4" s="5" customFormat="1">
-      <c r="B2" s="13" t="s">
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" s="5" customFormat="1">
+      <c r="A2" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="13"/>
-    </row>
-    <row r="3" spans="2:4" s="3" customFormat="1">
-      <c r="B3" s="11" t="s">
+      <c r="B2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" s="3" customFormat="1">
+      <c r="A3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="14" t="s">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="11" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="11" t="s">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="11" t="s">
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="11" t="s">
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="11" t="s">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="10" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="11" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="11" t="s">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="11" t="s">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="14" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="10" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="11" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="11" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="11" t="s">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="11" t="s">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="11" t="s">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:4" s="5" customFormat="1">
-      <c r="B25" s="10" t="s">
+    <row r="25" spans="1:3" s="5" customFormat="1">
+      <c r="A25" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="11" t="s">
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="11" t="s">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="11" t="s">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="7" t="s">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="14" t="s">
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="10" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="11" t="s">
+      <c r="B31" s="10"/>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="11" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="11" t="s">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="7" t="s">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="11" t="s">
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
-      <c r="B37" s="7" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="2:4">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="B38" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="2:4">
-      <c r="B39" s="11" t="s">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="1:3">
+      <c r="A40" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="B40" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="2:4">
-      <c r="B41" s="7" t="s">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="B42" s="14" t="s">
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
-      <c r="B43" s="10" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="2:4">
-      <c r="B44" s="11" t="s">
+      <c r="B43" s="10"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
-      <c r="B45" s="11" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="2:4">
-      <c r="B46" s="11" t="s">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="2:4">
-      <c r="B47" s="11" t="s">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="2:4">
-      <c r="B48" s="11" t="s">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
-      <c r="B49" s="7" t="s">
+    <row r="49" spans="1:3">
+      <c r="A49" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D49" s="5"/>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50" s="11" t="s">
+      <c r="C49" s="5"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="2:4">
-      <c r="B51" s="7" t="s">
+    <row r="51" spans="1:3">
+      <c r="A51" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D51" s="5"/>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="B52" s="14" t="s">
+      <c r="C51" s="5"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
fixed pdf, rm epub, bookdown file cleanup
</commit_message>
<xml_diff>
--- a/data/agenda.xlsx
+++ b/data/agenda.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="4380" yWindow="0" windowWidth="22320" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,20 +61,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Departure to the Centro de Biologia Marinha (CEBIMar) in São Sebastião</t>
   </si>
   <si>
-    <t>Open computer lab work</t>
-  </si>
-  <si>
     <t>Adjourn</t>
   </si>
   <si>
-    <t>Opening of AmeriGEOSS Week at the Instituto Nacional de Pesquisas Espaciais (INPE; São José dos Campos) [Gutierrez, Montes]</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -166,6 +160,9 @@
   </si>
   <si>
     <t>- Integrated visualization of OBIS records and satellite data</t>
+  </si>
+  <si>
+    <t>Opening of AmeriGEOSS Week at the Instituto Nacional de Pesquisas Espaciais (INPE; São José dos Campos)</t>
   </si>
 </sst>
 </file>
@@ -300,15 +297,15 @@
     <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -669,289 +666,289 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.6640625" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1">
       <c r="A1" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" s="5" customFormat="1">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" s="5" customFormat="1">
-      <c r="A2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1">
       <c r="A3" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="13"/>
+      <c r="A5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="10"/>
-      <c r="B7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="14"/>
+      <c r="B7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="10"/>
-      <c r="B8" s="16" t="s">
-        <v>12</v>
+      <c r="B8" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" s="5" customFormat="1">
       <c r="A9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="10"/>
-      <c r="B10" s="17" t="s">
-        <v>14</v>
+      <c r="B10" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="10"/>
-      <c r="B11" s="16" t="s">
-        <v>15</v>
+      <c r="B11" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
+      <c r="B12" s="13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="13"/>
+      <c r="A13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="17"/>
       <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" s="5" customFormat="1">
       <c r="A15" s="10"/>
-      <c r="B15" s="16" t="s">
-        <v>17</v>
+      <c r="B15" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="10"/>
-      <c r="B16" s="16" t="s">
-        <v>18</v>
+      <c r="B16" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="10"/>
-      <c r="B17" s="16" t="s">
-        <v>12</v>
+      <c r="B17" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1">
       <c r="A18" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="10"/>
-      <c r="B19" s="17" t="s">
-        <v>14</v>
+      <c r="B19" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="10"/>
-      <c r="B20" s="16" t="s">
-        <v>19</v>
+      <c r="B20" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="10"/>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="13"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="7"/>
-      <c r="B24" s="16" t="s">
-        <v>25</v>
+      <c r="B24" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="10"/>
-      <c r="B25" s="16" t="s">
-        <v>24</v>
+      <c r="B25" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="7"/>
-      <c r="B26" s="16" t="s">
-        <v>26</v>
+      <c r="B26" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" s="5" customFormat="1">
       <c r="A27" s="7"/>
-      <c r="B27" s="16" t="s">
-        <v>34</v>
+      <c r="B27" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="7"/>
-      <c r="B29" s="16" t="s">
-        <v>28</v>
+      <c r="B29" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="12"/>
-      <c r="B30" s="16" t="s">
-        <v>27</v>
+      <c r="B30" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1">
       <c r="A31" s="12"/>
-      <c r="B31" s="16" t="s">
-        <v>29</v>
+      <c r="B31" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="13"/>
+      <c r="A32" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="17"/>
       <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>31</v>
+        <v>6</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="10"/>
-      <c r="B34" s="16" t="s">
-        <v>32</v>
+      <c r="B34" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="7"/>
-      <c r="B35" s="16" t="s">
-        <v>33</v>
+      <c r="B35" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>